<commit_message>
More readable Excel Chart creation. Showed output to James.
</commit_message>
<xml_diff>
--- a/EarthquakeAnalysisTool/data.xlsx
+++ b/EarthquakeAnalysisTool/data.xlsx
@@ -13,6 +13,23 @@
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+  <si>
+    <t>time (s)</t>
+  </si>
+  <si>
+    <t>accel (g)</t>
+  </si>
+  <si>
+    <t>Surface</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -347,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -358,7 +375,30 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Calculate VTH and DTH from Surface and Base ATH
</commit_message>
<xml_diff>
--- a/EarthquakeAnalysisTool/data.xlsx
+++ b/EarthquakeAnalysisTool/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>time (s)</t>
   </si>
@@ -28,6 +28,15 @@
   </si>
   <si>
     <t>Base</t>
+  </si>
+  <si>
+    <t>accel (m/ss)</t>
+  </si>
+  <si>
+    <t>v (m/s)</t>
+  </si>
+  <si>
+    <t>d (m)</t>
   </si>
 </sst>
 </file>
@@ -37,8 +46,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,10 +83,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,42 +384,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="1" max="1" width="11" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" s="5" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" s="4"/>
+      <c r="H1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:12" s="5" customFormat="1">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>1</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>